<commit_message>
Results from R script
</commit_message>
<xml_diff>
--- a/Crédito disponível - Centralização - Campus Aracaju.xlsx
+++ b/Crédito disponível - Centralização - Campus Aracaju.xlsx
@@ -802,7 +802,9 @@
       <c r="M17" s="12">
         <v>57797.78</v>
       </c>
-      <c r="N17" s="12"/>
+      <c r="N17" s="12">
+        <v>3600</v>
+      </c>
       <c r="O17" s="13"/>
     </row>
     <row r="18">
@@ -852,7 +854,7 @@
         <v>21</v>
       </c>
       <c r="K19" s="12">
-        <v>47033.47</v>
+        <v>9738.95</v>
       </c>
       <c r="L19" s="12">
         <v>0</v>
@@ -1137,7 +1139,7 @@
         <v>106591.42</v>
       </c>
       <c r="N29" s="12">
-        <v>49077.69</v>
+        <v>51555.24</v>
       </c>
       <c r="O29" s="13">
         <v>49077.69</v>
@@ -1266,7 +1268,7 @@
         <v>485108.26</v>
       </c>
       <c r="O33" s="13">
-        <v>480428.26</v>
+        <v>481898.26</v>
       </c>
     </row>
     <row r="34">
@@ -1328,7 +1330,7 @@
         <v>122170</v>
       </c>
       <c r="O35" s="13">
-        <v>121790</v>
+        <v>122170</v>
       </c>
     </row>
     <row r="36">

</xml_diff>